<commit_message>
new script with unfiltered taxa
</commit_message>
<xml_diff>
--- a/SECPROD_SUMMARY_TOTALS.xlsx
+++ b/SECPROD_SUMMARY_TOTALS.xlsx
@@ -1,41 +1,78 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelleysinning/Library/CloudStorage/GoogleDrive-ksinning@vt.edu/My Drive/2023-2025 VT/Data/saltyC_VirginiaTech/SUMMARY SHEETS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelleysinning/Library/CloudStorage/GoogleDrive-ksinning@vt.edu/My Drive/2023-2025 VT/Data/SI_VT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD60EF19-01FD-4B47-BA20-E6B7B2C21E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB84951-D6D4-D94E-B93F-C0B4421EB4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="720" windowWidth="26080" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1460" yWindow="1700" windowWidth="26080" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SI available for top taxa" sheetId="14" r:id="rId1"/>
-    <sheet name="BOTTOM 5 FOR EACH STREAM" sheetId="13" r:id="rId2"/>
-    <sheet name="TOP 5 FOR EACH STREAM" sheetId="12" r:id="rId3"/>
-    <sheet name="TARGET TAXA CORE TOP 5" sheetId="6" r:id="rId4"/>
-    <sheet name="TARGET TAXA CORE BOTTOM 5" sheetId="7" r:id="rId5"/>
-    <sheet name="SI filtered for target taxa" sheetId="9" r:id="rId6"/>
-    <sheet name="TOTALS" sheetId="1" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId8"/>
-    <sheet name="TOP FFG for SI" sheetId="4" r:id="rId9"/>
-    <sheet name="BOTTOM FFG for SI" sheetId="5" r:id="rId10"/>
-    <sheet name="FFG" sheetId="2" r:id="rId11"/>
-    <sheet name="SITE SUMMARY" sheetId="3" r:id="rId12"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId13"/>
+    <sheet name="SI for ALL top taxa" sheetId="15" r:id="rId1"/>
+    <sheet name="SI for FILTERED top taxa" sheetId="14" r:id="rId2"/>
+    <sheet name="BOTTOM 5 FOR EACH STREAM" sheetId="13" r:id="rId3"/>
+    <sheet name="TOP 5 FOR EACH STREAM" sheetId="12" r:id="rId4"/>
+    <sheet name="TARGET TAXA CORE TOP 5" sheetId="6" r:id="rId5"/>
+    <sheet name="TARGET TAXA CORE BOTTOM 5" sheetId="7" r:id="rId6"/>
+    <sheet name="SI filtered for target taxa" sheetId="9" r:id="rId7"/>
+    <sheet name="TOTALS" sheetId="1" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId9"/>
+    <sheet name="TOP FFG for SI" sheetId="4" r:id="rId10"/>
+    <sheet name="BOTTOM FFG for SI" sheetId="5" r:id="rId11"/>
+    <sheet name="FFG" sheetId="2" r:id="rId12"/>
+    <sheet name="SITE SUMMARY" sheetId="3" r:id="rId13"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">TOTALS!$B$1:$B$519</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">TOTALS!$B$1:$B$519</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={BD3D543A-0072-054A-AA60-6EADF527EA72}</author>
+    <author>tc={CFCB5415-4547-E44D-985C-D6B79F5DC3F0}</author>
+    <author>tc={0B85926F-57C0-6C42-B0C4-367D902B1A6D}</author>
+  </authors>
+  <commentList>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{BD3D543A-0072-054A-AA60-6EADF527EA72}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    slightly different values from filtered, more data available for means</t>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="1" shapeId="0" xr:uid="{CFCB5415-4547-E44D-985C-D6B79F5DC3F0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    slightly different values from filtered, more data available for means</t>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="2" shapeId="0" xr:uid="{0B85926F-57C0-6C42-B0C4-367D902B1A6D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    slightly different values from filtered, but barely, more data available for means</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2571" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2665" uniqueCount="160">
   <si>
     <t>Genus</t>
   </si>
@@ -525,7 +562,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,6 +623,19 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -655,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -704,6 +754,10 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,6 +776,138 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EDF0540-B791-D24B-BA6A-34FB5B86F150}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="825500" y="4851400"/>
+          <a:ext cx="3962400" cy="3340100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Bold = top 5</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> taxa in production</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>italic = bottom 5 taxa in production</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>from next 2 tabs</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>filterSI.year1 in SI.Year1.UNFILTERED code, line 301</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>I reran the bottom and top taxa for all unfiltered macro year 1 data -- that is, it included the flawed data </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>There wasn't much of a difference when we included this, we only added representation from 1 shredder</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> in EAS that was low in production. The point of this would be to compare a low producing "sensitive??" shredder to others... but also Molophilus may not be that important to include</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Tallaperla, amphinemura, and tipula are only taxa that yielded different values with the additional inclusion of the unfiltered data</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -811,7 +997,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>filterSI.year1 in SI.Year1 code, line 281</a:t>
+            <a:t>filterSI.year1 in SI.Year1 code, line 294</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -822,7 +1008,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -918,7 +1104,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1009,7 +1195,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1098,7 +1284,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1206,7 +1392,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1294,7 +1480,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1383,7 +1569,9 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Sinning, Kelley" id="{C2F618E0-780F-0C46-828D-40804ACBADE9}" userId="S::ksinning@vt.edu::08d65797-bea8-41a3-b11b-f54549a403af" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1671,746 +1859,965 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D7" dT="2025-09-28T22:18:17.10" personId="{C2F618E0-780F-0C46-828D-40804ACBADE9}" id="{BD3D543A-0072-054A-AA60-6EADF527EA72}">
+    <text>slightly different values from filtered, more data available for means</text>
+  </threadedComment>
+  <threadedComment ref="D8" dT="2025-09-28T22:18:35.41" personId="{C2F618E0-780F-0C46-828D-40804ACBADE9}" id="{CFCB5415-4547-E44D-985C-D6B79F5DC3F0}">
+    <text>slightly different values from filtered, more data available for means</text>
+  </threadedComment>
+  <threadedComment ref="D22" dT="2025-09-28T22:19:20.07" personId="{C2F618E0-780F-0C46-828D-40804ACBADE9}" id="{0B85926F-57C0-6C42-B0C4-367D902B1A6D}">
+    <text>slightly different values from filtered, but barely, more data available for means</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5507C41A-FCCC-ED40-9319-C4766F921F86}">
-  <dimension ref="A1:L22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44FC0A3-D1D8-9A4A-89E2-C2A77A23CA5B}">
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14" t="s">
+      <c r="I1" s="9"/>
+      <c r="J1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="9" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="2">
         <v>5.5533330000000003</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="2">
         <v>44.003329999999998</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="2">
         <v>9.5333330000000007</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="2">
         <v>-0.71666669999999999</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="2">
         <v>-28.183330000000002</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2">
         <v>16</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+    </row>
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="2">
         <v>10.43</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="2">
         <v>51.42</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="2">
         <v>5.75</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="2">
         <v>0.78</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="2">
         <v>-32.880000000000003</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2">
         <v>16</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+    </row>
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="2">
+        <v>10.29</v>
+      </c>
+      <c r="E4" s="2">
+        <v>53.19</v>
+      </c>
+      <c r="F4" s="2">
+        <v>6.03</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.43</v>
+      </c>
+      <c r="H4" s="2">
+        <v>-27.86</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2">
+        <v>16</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C5" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D5" s="2">
         <v>9.4570830000000008</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E5" s="2">
         <v>50.095829999999999</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F5" s="2">
         <v>7.0894440000000003</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G5" s="2">
         <v>-0.18458330000000001</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H5" s="2">
         <v>-27.558330000000002</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
         <v>16</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K5" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+    </row>
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B6" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C6" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D6" s="2">
         <v>7.5949999999999998</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E6" s="2">
         <v>44.005000000000003</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F6" s="2">
         <v>6.915</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G6" s="2">
         <v>1.76</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H6" s="2">
         <v>-27.625</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
         <v>16</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K6" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="L5" s="5"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+    </row>
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B7" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C7" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="10">
-        <v>12.11</v>
-      </c>
-      <c r="E6" s="10">
-        <v>56.61</v>
-      </c>
-      <c r="F6" s="10">
+      <c r="D7" s="2">
+        <v>11.3125</v>
+      </c>
+      <c r="E7" s="2">
+        <v>55.945</v>
+      </c>
+      <c r="F7" s="2">
         <v>7.06</v>
       </c>
-      <c r="G6" s="10">
-        <v>1.3966666999999999</v>
-      </c>
-      <c r="H6" s="10">
-        <v>-27.63</v>
-      </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10">
+      <c r="G7" s="2">
+        <v>1.2324999999999999</v>
+      </c>
+      <c r="H7" s="2">
+        <v>-27.782499999999999</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2">
         <v>16</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K7" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+    </row>
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B8" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C8" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="10">
-        <v>10.72</v>
-      </c>
-      <c r="E7" s="10">
-        <v>47.25</v>
-      </c>
-      <c r="F7" s="10">
-        <v>5.14</v>
-      </c>
-      <c r="G7" s="10">
-        <v>0.93</v>
-      </c>
-      <c r="H7" s="10">
-        <v>-26.63</v>
-      </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10">
+      <c r="D8" s="2">
+        <v>9.2050000000000001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>43.52</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5.585</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="H8" s="2">
+        <v>-26.524999999999999</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2">
         <v>350</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K8" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="L7" s="5"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+    </row>
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B9" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C9" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D9" s="2">
         <v>7.7175000000000002</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E9" s="2">
         <v>47.517499999999998</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F9" s="2">
         <v>7.5374999999999996</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G9" s="2">
         <v>3.1724999999999999</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H9" s="2">
         <v>-25.807500000000001</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2">
         <v>350</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K9" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="L8" s="5"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+    </row>
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B10" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C10" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D10" s="2">
         <v>8.8825000000000003</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E10" s="2">
         <v>47.427500000000002</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F10" s="2">
         <v>6.2350000000000003</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G10" s="2">
         <v>2.19</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H10" s="2">
         <v>-25.612500000000001</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10">
+      <c r="I10" s="2"/>
+      <c r="J10" s="2">
         <v>350</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K10" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+    </row>
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B11" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C11" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D11" s="2">
         <v>10.1</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E11" s="2">
         <v>47.2</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F11" s="2">
         <v>5.45</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G11" s="2">
         <v>-0.34</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H11" s="2">
         <v>-30.94</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2">
         <v>350</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="L10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+    </row>
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B12" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C12" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D12" s="2">
         <v>9.3668750000000003</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E12" s="2">
         <v>47.361249999999998</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F12" s="2">
         <v>6.3766670000000003</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G12" s="2">
         <v>0.92343750000000002</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H12" s="2">
         <v>-27.11375</v>
       </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2">
         <v>350</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="K12" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+    </row>
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B13" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C13" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D13" s="2">
         <v>7.63</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E13" s="2">
         <v>41.35</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F13" s="2">
         <v>8.9</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G13" s="2">
         <v>5.7925000000000004</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H13" s="2">
         <v>-28.377500000000001</v>
       </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
         <v>350</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K13" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+    </row>
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B14" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C14" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D14" s="2">
         <v>11.29</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E14" s="2">
         <v>49.2</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F14" s="2">
         <v>5.08</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G14" s="2">
         <v>2.88</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H14" s="2">
         <v>-26.09</v>
       </c>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2">
         <v>350</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K14" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="L13" s="5"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+    </row>
+    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B15" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C15" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D15" s="2">
         <v>9.9433330000000009</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E15" s="2">
         <v>42.266669999999998</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F15" s="2">
         <v>5.2149999999999999</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G15" s="2">
         <v>1.7983332999999999</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H15" s="2">
         <v>-26.65</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2">
         <v>350</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="K15" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="L14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
+    </row>
+    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B16" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C16" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D16" s="2">
         <v>8.8550000000000004</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E16" s="2">
         <v>43.82</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F16" s="2">
         <v>5.85</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G16" s="2">
         <v>6.66</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H16" s="2">
         <v>-23.125</v>
       </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2">
         <v>1185</v>
       </c>
-      <c r="K15" s="10" t="s">
+      <c r="K16" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L15" s="5"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+    </row>
+    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B17" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C17" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D17" s="2">
         <v>10.81</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E17" s="2">
         <v>50.89</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F17" s="2">
         <v>5.49</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G17" s="2">
         <v>4.7</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H17" s="2">
         <v>-24.59</v>
       </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2">
         <v>1185</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="K17" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
+    </row>
+    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B18" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C18" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D18" s="2">
         <v>5</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E18" s="2">
         <v>43.31</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F18" s="2">
         <v>10.11</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G18" s="2">
         <v>0.7</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H18" s="2">
         <v>-28.69</v>
       </c>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10">
+      <c r="I18" s="2"/>
+      <c r="J18" s="2">
         <v>1185</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="K18" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
+    </row>
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B19" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C19" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D19" s="2">
         <v>6.648333</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E19" s="2">
         <v>48.891669999999998</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F19" s="2">
         <v>8.5983330000000002</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G19" s="2">
         <v>7.0883333000000004</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H19" s="2">
         <v>-25.406669999999998</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10">
+      <c r="I19" s="2"/>
+      <c r="J19" s="2">
         <v>1185</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K19" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
+    </row>
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B20" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C20" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D20" s="2">
         <v>8.65</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E20" s="2">
         <v>52.74</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F20" s="2">
         <v>7.11</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G20" s="2">
         <v>1.3</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H20" s="2">
         <v>-25.74</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10">
+      <c r="I20" s="2"/>
+      <c r="J20" s="2">
         <v>1185</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K20" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="s">
+    </row>
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B21" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C21" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D21" s="2">
         <v>9.2866669999999996</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E21" s="2">
         <v>47.536670000000001</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F21" s="2">
         <v>6.2466670000000004</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G21" s="2">
         <v>5.0033333000000004</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H21" s="2">
         <v>-27.246670000000002</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10">
+      <c r="I21" s="2"/>
+      <c r="J21" s="2">
         <v>1185</v>
       </c>
-      <c r="K20" s="10" t="s">
+      <c r="K21" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="25" t="s">
+    </row>
+    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B22" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C22" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D21" s="10">
-        <v>8.27</v>
-      </c>
-      <c r="E21" s="10">
-        <v>37.965000000000003</v>
-      </c>
-      <c r="F21" s="10">
-        <v>5.5575000000000001</v>
-      </c>
-      <c r="G21" s="10">
-        <v>2.1924999999999999</v>
-      </c>
-      <c r="H21" s="10">
-        <v>-27.5075</v>
-      </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10">
+      <c r="D22" s="2">
+        <v>8.59</v>
+      </c>
+      <c r="E22" s="2">
+        <v>39.178330000000003</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5.4716670000000001</v>
+      </c>
+      <c r="G22" s="2">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="H22" s="2">
+        <v>-27.483329999999999</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2">
         <v>1185</v>
       </c>
-      <c r="K21" s="10" t="s">
+      <c r="K22" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L21" s="5"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A33C90-033B-5C4D-B01D-3675459FD11C}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="3" max="3" width="31.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.918047473</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.65586213999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.38052138200000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8.8141790000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.07872E-4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.440221425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.30746790499999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.13406605299999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="2">
+        <v>7.3113448999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.6820681000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="2">
+        <v>23.28552517</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="2">
+        <v>8.7916209869999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6.7933530009999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2.104234725</v>
+      </c>
+      <c r="D15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.1324433679999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2418,7 +2825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752D9365-6A36-C84A-A0B9-F72E8B49CB15}">
   <dimension ref="A1:I17"/>
   <sheetViews>
@@ -2697,7 +3104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C275A1-6111-5E45-9F34-48D990D918D8}">
   <dimension ref="A1:E55"/>
   <sheetViews>
@@ -3653,7 +4060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B8EA48-78B5-B149-A1BE-1DB6888D6347}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -3849,7 +4256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{959A572F-ED5D-8C4B-A3AA-52C1C7BDDF15}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3862,11 +4269,758 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5507C41A-FCCC-ED40-9319-C4766F921F86}">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="10">
+        <v>5.5533330000000003</v>
+      </c>
+      <c r="E2" s="10">
+        <v>44.003329999999998</v>
+      </c>
+      <c r="F2" s="10">
+        <v>9.5333330000000007</v>
+      </c>
+      <c r="G2" s="10">
+        <v>-0.71666669999999999</v>
+      </c>
+      <c r="H2" s="10">
+        <v>-28.183330000000002</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10">
+        <v>16</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="10">
+        <v>10.43</v>
+      </c>
+      <c r="E3" s="10">
+        <v>51.42</v>
+      </c>
+      <c r="F3" s="10">
+        <v>5.75</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0.78</v>
+      </c>
+      <c r="H3" s="10">
+        <v>-32.880000000000003</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10">
+        <v>16</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="10">
+        <v>9.4570830000000008</v>
+      </c>
+      <c r="E4" s="10">
+        <v>50.095829999999999</v>
+      </c>
+      <c r="F4" s="10">
+        <v>7.0894440000000003</v>
+      </c>
+      <c r="G4" s="10">
+        <v>-0.18458330000000001</v>
+      </c>
+      <c r="H4" s="10">
+        <v>-27.558330000000002</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10">
+        <v>16</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="10">
+        <v>7.5949999999999998</v>
+      </c>
+      <c r="E5" s="10">
+        <v>44.005000000000003</v>
+      </c>
+      <c r="F5" s="10">
+        <v>6.915</v>
+      </c>
+      <c r="G5" s="10">
+        <v>1.76</v>
+      </c>
+      <c r="H5" s="10">
+        <v>-27.625</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10">
+        <v>16</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="10">
+        <v>12.11</v>
+      </c>
+      <c r="E6" s="10">
+        <v>56.61</v>
+      </c>
+      <c r="F6" s="10">
+        <v>7.06</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1.3966666999999999</v>
+      </c>
+      <c r="H6" s="10">
+        <v>-27.63</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10">
+        <v>16</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="10">
+        <v>10.72</v>
+      </c>
+      <c r="E7" s="10">
+        <v>47.25</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5.14</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.93</v>
+      </c>
+      <c r="H7" s="10">
+        <v>-26.63</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10">
+        <v>350</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="10">
+        <v>7.7175000000000002</v>
+      </c>
+      <c r="E8" s="10">
+        <v>47.517499999999998</v>
+      </c>
+      <c r="F8" s="10">
+        <v>7.5374999999999996</v>
+      </c>
+      <c r="G8" s="10">
+        <v>3.1724999999999999</v>
+      </c>
+      <c r="H8" s="10">
+        <v>-25.807500000000001</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10">
+        <v>350</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="10">
+        <v>8.8825000000000003</v>
+      </c>
+      <c r="E9" s="10">
+        <v>47.427500000000002</v>
+      </c>
+      <c r="F9" s="10">
+        <v>6.2350000000000003</v>
+      </c>
+      <c r="G9" s="10">
+        <v>2.19</v>
+      </c>
+      <c r="H9" s="10">
+        <v>-25.612500000000001</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10">
+        <v>350</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="10">
+        <v>10.1</v>
+      </c>
+      <c r="E10" s="10">
+        <v>47.2</v>
+      </c>
+      <c r="F10" s="10">
+        <v>5.45</v>
+      </c>
+      <c r="G10" s="10">
+        <v>-0.34</v>
+      </c>
+      <c r="H10" s="10">
+        <v>-30.94</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10">
+        <v>350</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="10">
+        <v>9.3668750000000003</v>
+      </c>
+      <c r="E11" s="10">
+        <v>47.361249999999998</v>
+      </c>
+      <c r="F11" s="10">
+        <v>6.3766670000000003</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0.92343750000000002</v>
+      </c>
+      <c r="H11" s="10">
+        <v>-27.11375</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10">
+        <v>350</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="10">
+        <v>7.63</v>
+      </c>
+      <c r="E12" s="10">
+        <v>41.35</v>
+      </c>
+      <c r="F12" s="10">
+        <v>8.9</v>
+      </c>
+      <c r="G12" s="10">
+        <v>5.7925000000000004</v>
+      </c>
+      <c r="H12" s="10">
+        <v>-28.377500000000001</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10">
+        <v>350</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="10">
+        <v>11.29</v>
+      </c>
+      <c r="E13" s="10">
+        <v>49.2</v>
+      </c>
+      <c r="F13" s="10">
+        <v>5.08</v>
+      </c>
+      <c r="G13" s="10">
+        <v>2.88</v>
+      </c>
+      <c r="H13" s="10">
+        <v>-26.09</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10">
+        <v>350</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="10">
+        <v>9.9433330000000009</v>
+      </c>
+      <c r="E14" s="10">
+        <v>42.266669999999998</v>
+      </c>
+      <c r="F14" s="10">
+        <v>5.2149999999999999</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1.7983332999999999</v>
+      </c>
+      <c r="H14" s="10">
+        <v>-26.65</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10">
+        <v>350</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="10">
+        <v>8.8550000000000004</v>
+      </c>
+      <c r="E15" s="10">
+        <v>43.82</v>
+      </c>
+      <c r="F15" s="10">
+        <v>5.85</v>
+      </c>
+      <c r="G15" s="10">
+        <v>6.66</v>
+      </c>
+      <c r="H15" s="10">
+        <v>-23.125</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10">
+        <v>1185</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="10">
+        <v>10.81</v>
+      </c>
+      <c r="E16" s="10">
+        <v>50.89</v>
+      </c>
+      <c r="F16" s="10">
+        <v>5.49</v>
+      </c>
+      <c r="G16" s="10">
+        <v>4.7</v>
+      </c>
+      <c r="H16" s="10">
+        <v>-24.59</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10">
+        <v>1185</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="10">
+        <v>5</v>
+      </c>
+      <c r="E17" s="10">
+        <v>43.31</v>
+      </c>
+      <c r="F17" s="10">
+        <v>10.11</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="H17" s="10">
+        <v>-28.69</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10">
+        <v>1185</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="10">
+        <v>6.648333</v>
+      </c>
+      <c r="E18" s="10">
+        <v>48.891669999999998</v>
+      </c>
+      <c r="F18" s="10">
+        <v>8.5983330000000002</v>
+      </c>
+      <c r="G18" s="10">
+        <v>7.0883333000000004</v>
+      </c>
+      <c r="H18" s="10">
+        <v>-25.406669999999998</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10">
+        <v>1185</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="10">
+        <v>8.65</v>
+      </c>
+      <c r="E19" s="10">
+        <v>52.74</v>
+      </c>
+      <c r="F19" s="10">
+        <v>7.11</v>
+      </c>
+      <c r="G19" s="10">
+        <v>1.3</v>
+      </c>
+      <c r="H19" s="10">
+        <v>-25.74</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10">
+        <v>1185</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="10">
+        <v>9.2866669999999996</v>
+      </c>
+      <c r="E20" s="10">
+        <v>47.536670000000001</v>
+      </c>
+      <c r="F20" s="10">
+        <v>6.2466670000000004</v>
+      </c>
+      <c r="G20" s="10">
+        <v>5.0033333000000004</v>
+      </c>
+      <c r="H20" s="10">
+        <v>-27.246670000000002</v>
+      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10">
+        <v>1185</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" s="10">
+        <v>8.27</v>
+      </c>
+      <c r="E21" s="10">
+        <v>37.965000000000003</v>
+      </c>
+      <c r="F21" s="10">
+        <v>5.5575000000000001</v>
+      </c>
+      <c r="G21" s="10">
+        <v>2.1924999999999999</v>
+      </c>
+      <c r="H21" s="10">
+        <v>-27.5075</v>
+      </c>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10">
+        <v>1185</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C56EF8-60CC-504A-A1F2-BA3F73D9EB16}">
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="C32" sqref="C32:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4565,11 +5719,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E7045C-CED6-9348-82E8-F8C016D155D4}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="C32" sqref="C32:C45"/>
     </sheetView>
   </sheetViews>
@@ -5305,7 +6459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B115B9-9704-9946-AEF3-FEE71F271470}">
   <dimension ref="A1:I15"/>
   <sheetViews>
@@ -5553,7 +6707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E54C31-1B84-BE4F-9843-1710E1D324C0}">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -5759,7 +6913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9DE126-8408-4A4E-9083-A4456DC5D3AD}">
   <dimension ref="A1:K22"/>
   <sheetViews>
@@ -6470,7 +7624,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G519"/>
   <sheetViews>
@@ -18435,7 +19589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F5A4E6-6057-D245-B206-4BB3081263DD}">
   <dimension ref="A1:G69"/>
   <sheetViews>
@@ -20035,209 +21189,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A33C90-033B-5C4D-B01D-3675459FD11C}">
-  <dimension ref="A1:D16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="3" max="3" width="31.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.918047473</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.65586213999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.38052138200000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="2">
-        <v>8.8141790000000001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2.07872E-4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.440221425</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.30746790499999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.13406605299999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="2">
-        <v>7.3113448999999997E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1.6820681000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="2">
-        <v>23.28552517</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="2">
-        <v>8.7916209869999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2">
-        <v>6.7933530009999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="2">
-        <v>2.104234725</v>
-      </c>
-      <c r="D15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1.1324433679999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>